<commit_message>
final commits before Stellies
</commit_message>
<xml_diff>
--- a/case3_Borate/Excel_Files/Illovo_waste_water/_borate_PCR642Ca_Illovo.xlsx
+++ b/case3_Borate/Excel_Files/Illovo_waste_water/_borate_PCR642Ca_Illovo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\28820169\Desktop\MEng_Code\case3_Borate\Excel_Files\Illovo_waste_water\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1979230255d33e2/Desktop/MEng_Code/case3_Borate/Excel_Files/Illovo_waste_water/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FFB9A9-24DB-4C19-9E4A-4AE57D8841AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{C6FFB9A9-24DB-4C19-9E4A-4AE57D8841AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BD45811-45DC-4C97-8BA9-56CBD9600C59}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="glucose" sheetId="1" r:id="rId1"/>
@@ -2105,7 +2105,7 @@
   <dimension ref="A1:U68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2448,6 +2448,10 @@
         <v>1.535874E-3</v>
       </c>
       <c r="H8" s="2"/>
+      <c r="K8">
+        <f>K2*3.6</f>
+        <v>2.16</v>
+      </c>
     </row>
     <row r="9" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
@@ -3093,6 +3097,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010048117A934AEAC441AF47E945F1AED0C0" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7272456f5b53c8ae1c345851aef95d27">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c39f1452-4462-4979-941b-c1317cfd14ce" xmlns:ns3="60199b31-2299-4531-8872-a3eaba744cbd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="16ed4d68a838bfbb08a7468a1792fb8f" ns2:_="" ns3:_="">
     <xsd:import namespace="c39f1452-4462-4979-941b-c1317cfd14ce"/>
@@ -3349,16 +3362,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21AAFDFA-AF70-4552-A086-9BCC58150335}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF42137A-B7F2-4A60-BAD9-4B8683F12BBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3375,12 +3387,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21AAFDFA-AF70-4552-A086-9BCC58150335}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>